<commit_message>
added a fold_loop and a cross_validation functions in cross_validation.py
</commit_message>
<xml_diff>
--- a/hyperparameters_choice.xlsx
+++ b/hyperparameters_choice.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etien\Repositories\images_hyperspectrales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAF766D-5DCD-4E31-9B4A-27DF705EFF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE9F982-4AE7-4660-97A3-591762880F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{952C5C7E-0D03-4DC7-A1DE-62262F97FA6C}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{952C5C7E-0D03-4DC7-A1DE-62262F97FA6C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CNN_1" sheetId="1" r:id="rId1"/>
+    <sheet name="CNN_2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
   <si>
     <t>H_1</t>
   </si>
@@ -56,14 +57,44 @@
     <t>conv</t>
   </si>
   <si>
-    <t>pool</t>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>in_channels</t>
+  </si>
+  <si>
+    <t>out_channels</t>
+  </si>
+  <si>
+    <t>bands</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n_param</t>
+  </si>
+  <si>
+    <t>n_tot</t>
+  </si>
+  <si>
+    <t>H_pool</t>
+  </si>
+  <si>
+    <t>kernel_pool</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,13 +102,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,8 +137,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,122 +463,669 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57DB373-2147-45FB-81EC-C1A11C43C97C}">
-  <dimension ref="A2:F8"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2">
+        <v>200</v>
+      </c>
+      <c r="G2" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H6" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="I6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <f>(C3-D3+2*E3)/F3+1</f>
+      <c r="B7" s="2">
+        <f>D7/C7</f>
+        <v>100</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <f>(E7-F7+2*G7)/H7+1</f>
+        <v>200</v>
+      </c>
+      <c r="E7" s="2">
+        <v>200</v>
+      </c>
+      <c r="F7" s="4">
+        <v>7</v>
+      </c>
+      <c r="G7" s="4">
+        <v>3</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="J7" s="4">
+        <f>E2</f>
+        <v>3</v>
+      </c>
+      <c r="K7" s="2">
+        <f>(F7*F7*J7+1)*I7</f>
+        <v>1480</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ref="L7:L8" si="0">K7/$B$12</f>
+        <v>8.9730686682268496E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" ref="B8:B9" si="1">D8/C8</f>
+        <v>50</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <f>(E8-F8+2*G8)/H8+1</f>
+        <v>100</v>
+      </c>
+      <c r="E8" s="2">
+        <f>B7</f>
+        <v>100</v>
+      </c>
+      <c r="F8" s="4">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
+        <v>15</v>
+      </c>
+      <c r="J8" s="4">
+        <f>I7</f>
+        <v>10</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" ref="K8" si="2">(F8*F8*J8+1)*I8</f>
+        <v>3765</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>2.2826759145860871E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <f>(E9-F9+2*G9)/H9+1</f>
+        <v>50</v>
+      </c>
+      <c r="E9" s="2">
+        <f>B8</f>
+        <v>50</v>
+      </c>
+      <c r="F9" s="4">
+        <v>3</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
+        <v>25</v>
+      </c>
+      <c r="J9" s="4">
+        <f>I8</f>
+        <v>15</v>
+      </c>
+      <c r="K9" s="2">
+        <f>(F9*F9*J9+1)*I9</f>
+        <v>3400</v>
+      </c>
+      <c r="L9">
+        <f>K9/$B$12</f>
+        <v>2.0613806399980599E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="4">
+        <v>10</v>
+      </c>
+      <c r="J10" s="2">
+        <f>I9*B9*B9</f>
+        <v>15625</v>
+      </c>
+      <c r="K10" s="2">
+        <f>I10*(J10+1)</f>
+        <v>156260</v>
+      </c>
+      <c r="L10">
+        <f>K10/$B$12</f>
+        <v>0.94738629060616719</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2">
+        <v>3</v>
+      </c>
+      <c r="J11" s="4">
+        <f>I10</f>
+        <v>10</v>
+      </c>
+      <c r="K11" s="2">
+        <f>I11*(J11+1)</f>
+        <v>33</v>
+      </c>
+      <c r="L11">
+        <f>K11/$B$12</f>
+        <v>2.0007517976451759E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3">
+        <f>SUM(K7:K11)</f>
+        <v>164938</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC17E4D-D943-4ED2-97CE-AF741A99E83F}">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>216</v>
+      </c>
+      <c r="F2" s="2">
+        <v>200</v>
+      </c>
+      <c r="G2" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <f>D7/C7</f>
         <v>66</v>
       </c>
-      <c r="C3">
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <f>(E7-F7+2*G7)/H7+1</f>
+        <v>198</v>
+      </c>
+      <c r="E7" s="2">
         <v>200</v>
       </c>
-      <c r="D3">
+      <c r="F7" s="4">
+        <v>7</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
+        <f>E2</f>
+        <v>216</v>
+      </c>
+      <c r="J7" s="4">
+        <v>8</v>
+      </c>
+      <c r="K7" s="2">
+        <f>(F7*F7*I7+1)*J7</f>
+        <v>84680</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ref="L7:L14" si="0">K7/$B$15</f>
+        <v>0.21612626592616793</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="B8" s="2">
+        <f t="shared" ref="B8:B9" si="1">D8/C8</f>
+        <v>32</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <f>(E8-F8+2*G8)/H8+1</f>
+        <v>64</v>
+      </c>
+      <c r="E8" s="2">
+        <f>B7</f>
+        <v>66</v>
+      </c>
+      <c r="F8" s="4">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
+        <f>J7</f>
+        <v>8</v>
+      </c>
+      <c r="J8" s="4">
+        <v>16</v>
+      </c>
+      <c r="K8" s="2">
+        <f>(F8*F8*I8+1)*J8</f>
+        <v>3216</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>8.208101927474681E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <f>(E9-F9+2*G9)/H9+1</f>
+        <v>32</v>
+      </c>
+      <c r="E9" s="2">
+        <f>B8</f>
+        <v>32</v>
+      </c>
+      <c r="F9" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
+        <f>J8</f>
+        <v>16</v>
+      </c>
+      <c r="J9" s="4">
+        <v>32</v>
+      </c>
+      <c r="K9" s="2">
+        <f>(F9*F9*I9+1)*J9</f>
+        <v>4640</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>1.1842535119242078E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" ref="B10" si="2">D10/C10</f>
+        <v>8</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <f>(E10-F10+2*G10)/H10+1</f>
+        <v>16</v>
+      </c>
+      <c r="E10" s="2">
+        <f>B9</f>
+        <v>16</v>
+      </c>
+      <c r="F10" s="4">
+        <v>3</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4">
+        <f>J9</f>
+        <v>32</v>
+      </c>
+      <c r="J10" s="4">
+        <v>64</v>
+      </c>
+      <c r="K10" s="2">
+        <f>(F10*F10*I10+1)*J10</f>
+        <v>18496</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>4.7206795164978763E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" ref="B11" si="3">D11/C11</f>
+        <v>4</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <f>(E11-F11+2*G11)/H11+1</f>
+        <v>8</v>
+      </c>
+      <c r="E11" s="2">
+        <f>B10</f>
+        <v>8</v>
+      </c>
+      <c r="F11" s="4">
+        <v>3</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4">
+        <f>J10</f>
+        <v>64</v>
+      </c>
+      <c r="J11" s="4">
+        <v>128</v>
+      </c>
+      <c r="K11" s="2">
+        <f>(F11*F11*I11+1)*J11</f>
+        <v>73856</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0.18850049003593597</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <f>B3/2</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <f>(C5-D5+2*E5)/F5+1</f>
-        <v>18</v>
-      </c>
-      <c r="C5">
-        <f>B4</f>
-        <v>33</v>
-      </c>
-      <c r="D5">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2">
+        <f>J11*B11*B11</f>
+        <v>2048</v>
+      </c>
+      <c r="J12" s="4">
+        <v>100</v>
+      </c>
+      <c r="K12" s="2">
+        <f>J12*(I12+1)</f>
+        <v>204900</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0.52296022541653053</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="4">
+        <f>J12</f>
+        <v>100</v>
+      </c>
+      <c r="J13" s="2">
+        <v>20</v>
+      </c>
+      <c r="K13" s="2">
+        <f>J13*(I13+1)</f>
+        <v>2020</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>5.1555864096700429E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="4">
+        <f>J13</f>
+        <v>20</v>
+      </c>
+      <c r="J14" s="2">
         <v>3</v>
       </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <f>B5/2</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <f>(C7-D7+2*E7)/F7+1</f>
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <f>B6</f>
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <f>B7/2</f>
-        <v>3</v>
-      </c>
+      <c r="K14" s="2">
+        <f>J14*(I14+1)</f>
+        <v>63</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>1.6079304148970924E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <f>SUM(K7:K13)</f>
+        <v>391808</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>